<commit_message>
Reverted back removed coverage items
as for commit f7b50a26cad88741246c922a3fb9f56378fea400, some additions to XPULP vplan as random instruction generator will generate xpulp instructions on its own
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-immediate-branching.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-immediate-branching.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\xpulp_instruction_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C8C51E-D0F3-437D-AF95-4049F119B22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB90B802-8644-4ED3-9E47-58DB6E50A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3705" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
@@ -238,7 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,33 +283,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,25 +355,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -725,7 +709,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,43 +1109,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
-      <UserInfo>
-        <DisplayName>Pascal Gouedo</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Yoann Pruvost</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Xavier Aubert</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -1392,26 +1339,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
+      <UserInfo>
+        <DisplayName>Pascal Gouedo</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Yoann Pruvost</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Xavier Aubert</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0C40954-93D6-4BE1-9788-430B4983669A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A18C163-F09A-4423-B34F-E134654029BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62A6887-C1A7-4D38-9872-945F39256234}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1428,4 +1393,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A18C163-F09A-4423-B34F-E134654029BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0C40954-93D6-4BE1-9788-430B4983669A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
First batch of DV Plans annotations
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-immediate-branching.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-immediate-branching.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\xpulp_instruction_extensions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Simulation - Copie\xpulp_instruction_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB90B802-8644-4ED3-9E47-58DB6E50A8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252AF44F-D68A-4D9F-A919-C1780AF4B33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3705" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="5250" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="4" r:id="rId1"/>
     <sheet name="XPULP_IMM_BRANCHING" sheetId="1" r:id="rId2"/>
     <sheet name="DONOTDELETE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,6 +41,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={2BC348B3-9E44-48E8-9EBA-E8EFBD1505C5}</author>
+    <author>tc={3C8928CE-746A-4C0F-B7C8-086C1F3D23E3}</author>
+    <author>tc={7CA8A374-4E75-4230-A024-404E417A9CFE}</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0" shapeId="0" xr:uid="{2BC348B3-9E44-48E8-9EBA-E8EFBD1505C5}">
@@ -51,12 +53,28 @@
     Thanks to Vaibhav and Pascal comments, this part is in fact not relevant as immediate branching is totally verified in formal (SAIL description misreading on my side) </t>
       </text>
     </comment>
+    <comment ref="J4" authorId="1" shapeId="0" xr:uid="{3C8928CE-746A-4C0F-B7C8-086C1F3D23E3}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    missing</t>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="2" shapeId="0" xr:uid="{7CA8A374-4E75-4230-A024-404E417A9CFE}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    missing</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -127,9 +145,6 @@
 rs1 equal to imm5 (0)</t>
   </si>
   <si>
-    <t>CV32E40P User Manual - Chapter 18.4.6 Immediate Branching Operations</t>
-  </si>
-  <si>
     <t>Self Checking Test</t>
   </si>
   <si>
@@ -173,33 +188,6 @@
   </si>
   <si>
     <t>ENV capability, not specific test</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This verification plan is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NOT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> intended to be considered complete nor standalone. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">It is covering all the missing feature that formal verification was not able to verify for various reasons (complexity, run time, …) </t>
   </si>
   <si>
     <t xml:space="preserve">Please also refer to the corresponding Formal Verification Plans to have a complete view on what is verified. </t>
@@ -233,26 +221,58 @@
   <si>
     <t>Branch to PC + (imm12 &lt;&lt; 1) if rs1!=Imm5. Imm5 is signed</t>
   </si>
+  <si>
+    <t>Link to Coverage</t>
+  </si>
+  <si>
+    <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_beqimm_cg.cp_rs1_sign.pos
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_beqimm_cg.cp_rs1_sign.neg
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_beqimm_cg.cp_rs1_maxvals.zero</t>
+  </si>
+  <si>
+    <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_beqimm_cg.cp_imm5_sign.pos
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_beqimm_cg.cp_imm5_sign.neg</t>
+  </si>
+  <si>
+    <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_bneimm_cg.cp_rs1_sign.pos
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_bneimm_cg.cp_rs1_sign.neg
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_bneimm_cg.cp_rs1_maxvals.zero</t>
+  </si>
+  <si>
+    <t>CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_bneimm_cg.cp_imm5_sign.pos
+CG: RISCV_coverage_pkg.RISCV_coverage__1.cv_bneimm_cg.cp_imm5_sign.neg</t>
+  </si>
+  <si>
+    <t>Related Test Program(s)</t>
+  </si>
+  <si>
+    <t>corev_rand_pulp_instr_test
+pulp_immediate_branching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some information in this verification plan are meant to be complementary to formal verification verification plans, in order to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cover all the missing feature that formal verification was not able to verify for various reasons (complexity, run time, …) </t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>CV32E40P User Manual - Chapter 7.5.6 Immediate Branching Operations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -271,12 +291,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -289,6 +303,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -321,29 +343,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -355,26 +367,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -666,6 +690,12 @@
   <threadedComment ref="A2" dT="2023-02-27T09:14:32.94" personId="{90C50104-7037-45DE-94E3-964203FCE81D}" id="{2BC348B3-9E44-48E8-9EBA-E8EFBD1505C5}">
     <text xml:space="preserve">Thanks to Vaibhav and Pascal comments, this part is in fact not relevant as immediate branching is totally verified in formal (SAIL description misreading on my side) </text>
   </threadedComment>
+  <threadedComment ref="J4" dT="2024-03-01T09:12:38.00" personId="{90C50104-7037-45DE-94E3-964203FCE81D}" id="{3C8928CE-746A-4C0F-B7C8-086C1F3D23E3}">
+    <text>missing</text>
+  </threadedComment>
+  <threadedComment ref="J7" dT="2024-03-01T09:12:42.56" personId="{90C50104-7037-45DE-94E3-964203FCE81D}" id="{7CA8A374-4E75-4230-A024-404E417A9CFE}">
+    <text>missing</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -674,28 +704,28 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="114.85546875" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="114.85546875" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>35</v>
+      <c r="A1" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>36</v>
+      <c r="A2" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>37</v>
+      <c r="A3" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -706,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,268 +748,311 @@
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="5" max="6" width="41.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="106.42578125" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="J1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="F2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="19" t="s">
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="19" t="s">
+      <c r="J3" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="19" t="s">
+      <c r="J5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I6" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="19" t="s">
+      <c r="J6" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -1005,101 +1078,101 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="8"/>
-    <col min="3" max="3" width="26.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="8"/>
-    <col min="5" max="5" width="19.28515625" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="17.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="4"/>
+    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="4"/>
+    <col min="5" max="5" width="19.28515625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="8" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
-        <v>32</v>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1109,6 +1182,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -1339,15 +1421,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1377,6 +1450,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A18C163-F09A-4423-B34F-E134654029BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62A6887-C1A7-4D38-9872-945F39256234}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1395,14 +1476,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A18C163-F09A-4423-B34F-E134654029BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0C40954-93D6-4BE1-9788-430B4983669A}">
   <ds:schemaRefs>

</xml_diff>